<commit_message>
Transfer from Google drive
</commit_message>
<xml_diff>
--- a/data/final_values.xlsx
+++ b/data/final_values.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a1f71d1887b83a8d/Documents/Uni/ISM/ETF_python/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{394776EA-21C1-4726-BA09-E6080FF7610A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D85E7E69-EB68-4392-B1AF-90F89196A2FE}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{394776EA-21C1-4726-BA09-E6080FF7610A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20271A48-6B10-4CC3-A6B7-ABD56EEB7C0C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{136D3A7A-EF00-4769-9EE5-EB3247066080}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{136D3A7A-EF00-4769-9EE5-EB3247066080}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -24,9 +25,32 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="6">
+  <si>
+    <t>this chart is roughly consistent with high risk high return and vice versa. Because the high return parts have have lower 1 percentiles</t>
+  </si>
+  <si>
+    <t>US_5001440</t>
+  </si>
+  <si>
+    <t>CHINA_A501440</t>
+  </si>
+  <si>
+    <t>DAX301440</t>
+  </si>
+  <si>
+    <t>GOLD1440</t>
+  </si>
+  <si>
+    <t>SILVER1440</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -41,6 +65,18 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -66,12 +102,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2196,7 +2233,357 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$1:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.1161766782895199</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.15698233837196</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0733518802956401</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0830950466339899</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1147973103225099</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.91259726008225395</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71067043232947402</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78577630762869499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.88609954641712096</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.79939055565634198</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F644-4838-8CFC-894066B791D4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2034592351"/>
+        <c:axId val="2034591519"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2034592351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2034591519"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2034591519"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2034592351"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2752,6 +3139,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2773,6 +3676,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D2E222D-52BE-41F6-A361-51830FC2070F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A4B91A3-13C1-47E7-A252-C9263CCF5B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3092,7 +4036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C448EE32-F064-4A8C-9ED1-0CE065493283}">
   <dimension ref="A1:B300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A270" workbookViewId="0">
+    <sheetView topLeftCell="A270" workbookViewId="0">
       <selection sqref="A1:B300"/>
     </sheetView>
   </sheetViews>
@@ -5503,4 +6447,153 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88CF48EB-B1DF-467A-9979-428FB9F3A102}">
+  <dimension ref="A1:D31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3">
+        <v>1.1161766782895199</v>
+      </c>
+      <c r="B1" s="3">
+        <v>0.91259726008225395</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1.15698233837196</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.71067043232947402</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>1.0733518802956401</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.78577630762869499</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>1.0830950466339899</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.88609954641712096</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>1.1147973103225099</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.79939055565634198</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>1.0990260940857199</v>
+      </c>
+      <c r="D22">
+        <v>0.82374165863925297</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>